<commit_message>
Cập nhật  tiến độ công việc làm jwt service
</commit_message>
<xml_diff>
--- a/LmsMini.Resources/File kế hoạch gantt/gantt_tổng_có_giao_diện_lẫn_back_end.xlsx
+++ b/LmsMini.Resources/File kế hoạch gantt/gantt_tổng_có_giao_diện_lẫn_back_end.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Blazor\LmsMini\LmsMini.Resources\File kế hoạch gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0919D8-9BEF-4F5C-B326-9491E1561EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3505EF-E78C-4A70-99EC-07B619906A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="14" r:id="rId1"/>
@@ -3515,7 +3515,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{62B8AC4B-1E99-4FB3-A2FC-BD32F875A08D}" type="CELLRANGE">
+                    <a:fld id="{7D53BCE8-19E4-49FA-B274-3FB1C5B7A357}" type="CELLRANGE">
                       <a:rPr lang="vi-VN"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3549,7 +3549,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D0DF0C4-D2BE-4AD4-884B-6E6A10313030}" type="CELLRANGE">
+                    <a:fld id="{B59B046F-722E-4863-9E50-585451BE4544}" type="CELLRANGE">
                       <a:rPr lang="vi-VN"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3583,7 +3583,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35B22235-BBAF-410A-A053-D1C5A47D6260}" type="CELLRANGE">
+                    <a:fld id="{B0173380-C050-41C5-8B39-40C9F6CDEC63}" type="CELLRANGE">
                       <a:rPr lang="vi-VN"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3617,7 +3617,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD6AB624-2CEE-48D3-8F0C-B1FBDE7FA444}" type="CELLRANGE">
+                    <a:fld id="{58EC5A22-02F2-454C-987C-EFB3A043F6CA}" type="CELLRANGE">
                       <a:rPr lang="vi-VN"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3651,7 +3651,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6CE732DF-D704-4F94-8517-32576F0FDED5}" type="CELLRANGE">
+                    <a:fld id="{811E437D-8584-4475-9B4D-D5194FDD6F0C}" type="CELLRANGE">
                       <a:rPr lang="vi-VN"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3685,7 +3685,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AAF9AC20-4379-433E-BC8A-B06A3302A30A}" type="CELLRANGE">
+                    <a:fld id="{D97F57E4-4ABE-4DD3-AAA9-6412D600427A}" type="CELLRANGE">
                       <a:rPr lang="vi-VN"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3719,7 +3719,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6CA12DC2-2D52-42E9-A824-AEA4523B31C2}" type="CELLRANGE">
+                    <a:fld id="{1D441C20-8069-4DF8-AAF5-647E05F74E3D}" type="CELLRANGE">
                       <a:rPr lang="vi-VN"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5267,7 +5267,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -7664,8 +7664,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8055,7 +8055,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>9</v>
+        <v>332</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>102</v>

</xml_diff>